<commit_message>
Add product-list, product-show page
</commit_message>
<xml_diff>
--- a/Json file for categories.xlsx
+++ b/Json file for categories.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Siddhvastu5.com\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\11ty\Siddhvastu5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16600" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16600" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Categories" sheetId="1" r:id="rId1"/>
+    <sheet name="Products" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -162,6 +163,42 @@
   </si>
   <si>
     <t>/assets/imgs/shop/consultancy.png</t>
+  </si>
+  <si>
+    <t>product id</t>
+  </si>
+  <si>
+    <t>product name</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Categories id</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>Content</t>
   </si>
 </sst>
 </file>
@@ -496,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="B3:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -822,4 +859,118 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.90625" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>